<commit_message>
new exe version and parameter doc
</commit_message>
<xml_diff>
--- a/docs/VarroaPop Exposed Parameter List.xlsx
+++ b/docs/VarroaPop Exposed Parameter List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="239">
   <si>
     <t>Type</t>
   </si>
@@ -186,9 +186,6 @@
     <t>DEPesticide</t>
   </si>
   <si>
-    <t>Enumerated</t>
-  </si>
-  <si>
     <t>TotalImmMites</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Any valid</t>
-  </si>
-  <si>
     <t>ImmType</t>
   </si>
   <si>
@@ -448,6 +442,300 @@
   </si>
   <si>
     <t>Internal Associated Variable</t>
+  </si>
+  <si>
+    <t>Valid strings are: None, Sine, Cosine, Tangent, Exponential, Logarithmic, Polynomial</t>
+  </si>
+  <si>
+    <t>1/1/100</t>
+  </si>
+  <si>
+    <t>Commonly used date strings.</t>
+  </si>
+  <si>
+    <t>Unused</t>
+  </si>
+  <si>
+    <t>Min/Max from Kris' email 8/29/2014</t>
+  </si>
+  <si>
+    <t>Max value only constrained by data type</t>
+  </si>
+  <si>
+    <t>Min/Max value only constrained by data type</t>
+  </si>
+  <si>
+    <t>Absolute file path</t>
+  </si>
+  <si>
+    <t>Interpretation</t>
+  </si>
+  <si>
+    <t>Location of weather file</t>
+  </si>
+  <si>
+    <t>Sets the start date of the simulation.  Must be within dates contained in weather file</t>
+  </si>
+  <si>
+    <t>Sets the end date of the simulation.  Must be within dates contained in weather file</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - # of drone adults</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - # of worker adults</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - # of drone brood</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - # of worker brood</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - # of drone larvae</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - # of worker larvae</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - # of drone eggs</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - # of worker eggs</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - forager lifespan in days</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - initial queen strenth. 1=weak, 5= string</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - % adult drones infested with varroa</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - number of mite offspring per infesting mite</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - % adult workers invested with varroa</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - % worker brood infested with varroa</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - % drone brood infested  with varroa</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - % of mites surviving and emerging from capped drone brood</t>
+  </si>
+  <si>
+    <t>Initial Conditions for simuation - % of mites surviving and emerging from capped worker brood</t>
+  </si>
+  <si>
+    <t>Plotting switches: true = no values plotted in output graph.</t>
+  </si>
+  <si>
+    <t>Plotting switches: true = Adult Drone quantities plotted in output graph.</t>
+  </si>
+  <si>
+    <t>Plotting switches: true = Adult Worker quantities plotted in output graph.</t>
+  </si>
+  <si>
+    <t>Plotting switches: true = Colony Size plotted in output graph.</t>
+  </si>
+  <si>
+    <t>Plotting switches: true = Drone Brood quantities plotted in output graph.</t>
+  </si>
+  <si>
+    <t>Plotting switches: true = Drone Egg quantities plotted in output graph.</t>
+  </si>
+  <si>
+    <t>Plotting switches: true = Drone Larvae quantities plotted in output graph.</t>
+  </si>
+  <si>
+    <t>Plotting switches: true = Forager quantities plotted in output graph.</t>
+  </si>
+  <si>
+    <t>Plotting switches: true = Total Mite quantities plotted in output graph.</t>
+  </si>
+  <si>
+    <t>Plotting switches: true = Mites in Drone Brood quantities plotted in output graph.</t>
+  </si>
+  <si>
+    <t>No Discrete Events - Clear any current</t>
+  </si>
+  <si>
+    <t>Discrete Event Swarm</t>
+  </si>
+  <si>
+    <t>Discrete Event Chalkbrood</t>
+  </si>
+  <si>
+    <t>Discrete Event Resource Depletion</t>
+  </si>
+  <si>
+    <t>Discrete Event Supercedure</t>
+  </si>
+  <si>
+    <t>Discrete Event Pesticide</t>
+  </si>
+  <si>
+    <t>Profile of immigration.  Total mites over timespan follow one of these curves</t>
+  </si>
+  <si>
+    <t>Total # mites immigrating into colony</t>
+  </si>
+  <si>
+    <t>% immigrating mites which are resistant to ?</t>
+  </si>
+  <si>
+    <t>Start Immigration</t>
+  </si>
+  <si>
+    <t>End Immigration</t>
+  </si>
+  <si>
+    <t>Enables or disables immigration</t>
+  </si>
+  <si>
+    <t>Delay in days after a requeening</t>
+  </si>
+  <si>
+    <t>Sets the date of requeening</t>
+  </si>
+  <si>
+    <t>Enables or disables requeening</t>
+  </si>
+  <si>
+    <t>Either establishes Schedule (true) or Automatic (false) requeening</t>
+  </si>
+  <si>
+    <t>Sets the strength of the requeened queen</t>
+  </si>
+  <si>
+    <t>Either establishes a single requeening (true) or requeening every year on this date(false)</t>
+  </si>
+  <si>
+    <t>Daily Pollen Consumption by age 4 Larvae</t>
+  </si>
+  <si>
+    <t>Daily Nectar Consumption by age 4 Larvae</t>
+  </si>
+  <si>
+    <t>Daily Pollen Consumption by age 5 Larvae</t>
+  </si>
+  <si>
+    <t>Daily Nectar Consumption by age 5 Larvae</t>
+  </si>
+  <si>
+    <t>Daily Pollen Consumption by Drone Larvae</t>
+  </si>
+  <si>
+    <t>Daily Nectar Consumption by Drone Larvae</t>
+  </si>
+  <si>
+    <t>Daily Pollen Consumption by age 1-3 Adult Workers</t>
+  </si>
+  <si>
+    <t>Daily Nectar Consumption by age 1-3 Adult Workers</t>
+  </si>
+  <si>
+    <t>Daily Pollen Consumption by age 4-10 Adult Workers</t>
+  </si>
+  <si>
+    <t>Daily Nectar Consumption by age 4-10 Adult Workers</t>
+  </si>
+  <si>
+    <t>Daily Pollen Consumption by age 11-20 Adult Workers</t>
+  </si>
+  <si>
+    <t>Daily Nectar Consumption by age 11-20 Adult Workers</t>
+  </si>
+  <si>
+    <t>Daily Pollen Consumption by Drone Adults</t>
+  </si>
+  <si>
+    <t>Daily Nectar Consumption by Drone Adults</t>
+  </si>
+  <si>
+    <t>Daily Pollen Consumption by Foragers</t>
+  </si>
+  <si>
+    <t>Daily Nectar Consumption by Foragers</t>
+  </si>
+  <si>
+    <t>Daily Nectar trips per Forager</t>
+  </si>
+  <si>
+    <t>Daily Pollen trips per Forager</t>
+  </si>
+  <si>
+    <t>Percent of all Foragers collecting Nectar</t>
+  </si>
+  <si>
+    <t>mg Pollen per forage trip per bee</t>
+  </si>
+  <si>
+    <t>mg Nectar per forager trip per bee</t>
+  </si>
+  <si>
+    <t>If true, enables foliar spray contamination mechanism</t>
+  </si>
+  <si>
+    <t>If true, enables soil contamination mechanism</t>
+  </si>
+  <si>
+    <t>If true, enables seed contamination mechanism</t>
+  </si>
+  <si>
+    <t>Foliar application date.</t>
+  </si>
+  <si>
+    <t>If true, enables the Nectar/Pollen Contamination file.</t>
+  </si>
+  <si>
+    <t>Name of the Nectar/Pollen Contamination file</t>
+  </si>
+  <si>
+    <t>Mass (grams) of colony Nectar resources at start of simulation</t>
+  </si>
+  <si>
+    <t>Mass (grams) of colony Pollen resources at start of simulation</t>
+  </si>
+  <si>
+    <t>Maximum mass (grams) of Nectar resources contained in colony during simulation</t>
+  </si>
+  <si>
+    <t>Maximum mass (grams) of Pollen resources contained in colony during simulation</t>
+  </si>
+  <si>
+    <t>If true, enables supplemental pollen feeding</t>
+  </si>
+  <si>
+    <t>Amount (grams) of pollen supplemental feed</t>
+  </si>
+  <si>
+    <t>Start date of pollen supplemental feeding</t>
+  </si>
+  <si>
+    <t>End date of pollen suppemental feeding</t>
+  </si>
+  <si>
+    <t>If true, enables supplemental nectar feeding</t>
+  </si>
+  <si>
+    <t>Amount (grams) of nectar supplemental feed</t>
+  </si>
+  <si>
+    <t>Start date of nectar supplemental feeding</t>
+  </si>
+  <si>
+    <t>End date of nectar suppemental feeding</t>
+  </si>
+  <si>
+    <t>Max proportion of total adult worker population that can be active foragers</t>
+  </si>
+  <si>
+    <t>If true, colony dies when pollen or nectar mass reaches 0</t>
   </si>
 </sst>
 </file>
@@ -496,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -511,6 +799,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -792,51 +1092,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130:G131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="37.62890625" style="3" customWidth="1"/>
     <col min="2" max="2" width="37.62890625" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83984375" style="3"/>
+    <col min="3" max="3" width="13.9453125" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.47265625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9.7890625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="87.734375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.83984375" style="3"/>
+    <col min="5" max="5" width="12.5234375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="42.62890625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="78.68359375" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.83984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" ht="17.7" x14ac:dyDescent="0.6">
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" ht="17.7" x14ac:dyDescent="0.6">
       <c r="A2" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G2" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -845,13 +1150,19 @@
         <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+        <v>58</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -860,13 +1171,19 @@
         <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+        <v>142</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -875,13 +1192,19 @@
         <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+        <v>142</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -892,8 +1215,14 @@
       <c r="D6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="F6" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -904,8 +1233,14 @@
       <c r="D7" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="F7" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -916,8 +1251,14 @@
       <c r="D8" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="F8" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -928,8 +1269,14 @@
       <c r="D9" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="F9" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -940,8 +1287,14 @@
       <c r="D10" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="F10" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -952,8 +1305,14 @@
       <c r="D11" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="F11" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -964,8 +1323,14 @@
       <c r="D12" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="F12" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -976,8 +1341,14 @@
       <c r="D13" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="F13" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -988,8 +1359,14 @@
       <c r="D14" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E14" s="4">
+        <v>5</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -997,8 +1374,17 @@
       <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="D15" s="4">
+        <v>4</v>
+      </c>
+      <c r="E15" s="4">
+        <v>16</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1009,8 +1395,14 @@
       <c r="D16" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E16" s="4">
+        <v>100</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1021,8 +1413,14 @@
       <c r="D17" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E17" s="4">
+        <v>100</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1033,8 +1431,11 @@
       <c r="D18" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="G18" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1045,8 +1446,14 @@
       <c r="D19" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E19" s="4">
+        <v>100</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1057,8 +1464,14 @@
       <c r="D20" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E20" s="4">
+        <v>100</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1069,8 +1482,14 @@
       <c r="D21" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E21" s="4">
+        <v>100</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1081,8 +1500,14 @@
       <c r="D22" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E22" s="4">
+        <v>100</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1093,8 +1518,14 @@
       <c r="D23" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E23" s="4">
+        <v>100</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1102,11 +1533,20 @@
       <c r="C24" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="D24" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="E24" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
+        <v>58</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1114,8 +1554,20 @@
       <c r="C25" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="D25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1123,8 +1575,20 @@
       <c r="C26" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="D26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1132,8 +1596,20 @@
       <c r="C27" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="D27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -1141,8 +1617,20 @@
       <c r="C28" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="D28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -1150,8 +1638,20 @@
       <c r="C29" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="D29" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1159,8 +1659,20 @@
       <c r="C30" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="D30" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1168,8 +1680,20 @@
       <c r="C31" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="D31" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -1177,8 +1701,20 @@
       <c r="C32" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D32" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -1186,8 +1722,20 @@
       <c r="C33" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D33" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -1195,8 +1743,20 @@
       <c r="C34" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D34" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -1204,8 +1764,20 @@
       <c r="C35" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D35" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -1213,8 +1785,20 @@
       <c r="C36" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D36" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -1222,8 +1806,20 @@
       <c r="C37" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D37" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1231,8 +1827,20 @@
       <c r="C38" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D38" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
         <v>45</v>
       </c>
@@ -1240,8 +1848,20 @@
       <c r="C39" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D39" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
         <v>46</v>
       </c>
@@ -1249,8 +1869,20 @@
       <c r="C40" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D40" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
         <v>47</v>
       </c>
@@ -1258,8 +1890,20 @@
       <c r="C41" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D41" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
         <v>48</v>
       </c>
@@ -1267,8 +1911,20 @@
       <c r="C42" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D42" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
         <v>49</v>
       </c>
@@ -1276,8 +1932,20 @@
       <c r="C43" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D43" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
@@ -1285,8 +1953,20 @@
       <c r="C44" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D44" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
         <v>51</v>
       </c>
@@ -1294,8 +1974,20 @@
       <c r="C45" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D45" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
         <v>52</v>
       </c>
@@ -1303,8 +1995,20 @@
       <c r="C46" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D46" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
         <v>53</v>
       </c>
@@ -1312,8 +2016,20 @@
       <c r="C47" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D47" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
@@ -1321,765 +2037,1525 @@
       <c r="C48" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D48" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A49" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A50" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A50" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A51" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D51" s="4">
+        <v>0</v>
+      </c>
+      <c r="E51" s="4">
+        <v>100</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A52" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D52" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E52" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A53" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D53" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E53" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A54" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D54" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A55" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D55" s="4">
+        <v>0</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D57" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E57" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A58" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D58" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A59" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D59" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A60" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D60" s="4">
+        <v>1</v>
+      </c>
+      <c r="E60" s="4">
+        <v>5</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A61" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D61" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A62" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D62" s="4">
+        <v>1</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A63" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D63" s="4">
+        <v>0</v>
+      </c>
+      <c r="E63" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A64" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D64" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A65" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D65" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E65" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A66" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A67" s="1"/>
+      <c r="D66" s="4">
+        <v>0</v>
+      </c>
+      <c r="E66" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A67" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="B67" s="1"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="C67" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" s="4">
+        <v>-9</v>
+      </c>
+      <c r="E67" s="4">
+        <v>-2</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A68" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D68" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="E68" s="4">
+        <v>100</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A69" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D69" s="4">
+        <v>-9</v>
+      </c>
+      <c r="E69" s="4">
+        <v>-2</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A70" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D70" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="E70" s="4">
+        <v>100</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A71" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D71" s="4">
+        <v>-9</v>
+      </c>
+      <c r="E71" s="4">
+        <v>-2</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A72" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D72" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="E72" s="4">
+        <v>100</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A73" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D73" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E73" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A74" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D74" s="4">
+        <v>1</v>
+      </c>
+      <c r="E74" s="4">
+        <v>10000</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A75" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D75" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E75" s="4">
+        <v>35</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A76" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="F76" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A77" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D77" s="4">
+        <v>0</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A78" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D78" s="4">
+        <v>0</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A79" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D79" s="4">
+        <v>0</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A80" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D80" s="4">
+        <v>0</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A81" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D81" s="4">
+        <v>0</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A82" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D82" s="4">
+        <v>0</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A83" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D83" s="4">
+        <v>0</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A84" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D84" s="4">
+        <v>0</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A85" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D85" s="4">
+        <v>0</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A86" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D86" s="4">
+        <v>0</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A87" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D87" s="4">
+        <v>0</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A88" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D88" s="4">
+        <v>0</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A89" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D89" s="4">
+        <v>0</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A90" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D90" s="4">
+        <v>0</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A91" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D91" s="4">
+        <v>0</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A92" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D92" s="4">
+        <v>0</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A93" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.5">
+        <v>22</v>
+      </c>
+      <c r="D93" s="4">
+        <v>0</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A94" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D94" s="4">
+        <v>0</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A95" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.5">
+        <v>23</v>
+      </c>
+      <c r="D95" s="4">
+        <v>0</v>
+      </c>
+      <c r="E95" s="4">
+        <v>100</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A96" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D96" s="4">
+        <v>0</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A97" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D97" s="4">
+        <v>0</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A98" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A99" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D99" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A100" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D100" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A101" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.5">
+        <v>23</v>
+      </c>
+      <c r="D101" s="4">
+        <v>0</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A102" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D102" s="4">
+        <v>0</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A103" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D103" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E103" s="4">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A104" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D104" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E104" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A105" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D105" s="4">
+        <v>0</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A106" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D106" s="4">
+        <v>0</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A107" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.5">
+        <v>21</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E107" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A108" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B108" s="1"/>
       <c r="C108" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D108" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E108" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A109" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D109" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E109" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A110" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D110" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E110" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A111" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D111" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E111" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A112" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D112" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E112" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A113" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D113" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E113" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A114" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A115" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.5">
+        <v>20</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A116" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.5">
+        <v>23</v>
+      </c>
+      <c r="D116" s="4">
+        <v>0</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A117" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B117" s="1"/>
       <c r="C117" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D117" s="4">
+        <v>0</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A118" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D118" s="4">
+        <v>0</v>
+      </c>
+      <c r="F118" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A119" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D119" s="4">
+        <v>0</v>
+      </c>
+      <c r="F119" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A120" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F120" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A121" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B121" s="1"/>
       <c r="C121" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.5">
+        <v>23</v>
+      </c>
+      <c r="D121" s="4">
+        <v>0</v>
+      </c>
+      <c r="F121" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A122" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B122" s="1"/>
       <c r="C122" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.5">
+        <v>21</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E122" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F122" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A123" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B123" s="1"/>
       <c r="C123" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D123" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E123" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A124" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F124" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A125" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.5">
+        <v>23</v>
+      </c>
+      <c r="D125" s="4">
+        <v>0</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A126" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.5">
+        <v>21</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E126" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F126" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A127" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D127" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E127" s="8">
+        <v>2958465</v>
+      </c>
+      <c r="F127" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A128" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B128" s="1"/>
       <c r="C128" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.5">
+        <v>23</v>
+      </c>
+      <c r="D128" s="4">
+        <v>0</v>
+      </c>
+      <c r="E128" s="4">
+        <v>1</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A129" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B129" s="1"/>
       <c r="C129" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A130" s="1" t="s">
-        <v>140</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F129" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A130" s="1"/>
       <c r="B130" s="1"/>
-      <c r="C130" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A131" s="1" t="s">
-        <v>129</v>
-      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A131" s="1"/>
       <c r="B131" s="1"/>
-      <c r="C131" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A132" s="1" t="s">
-        <v>130</v>
-      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A132" s="1"/>
       <c r="B132" s="1"/>
-      <c r="C132" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.5">
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A134" s="1"/>
-      <c r="B134" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated weather handling, testing 100k+ iterations
</commit_message>
<xml_diff>
--- a/docs/VarroaPop Exposed Parameter List.xlsx
+++ b/docs/VarroaPop Exposed Parameter List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="239">
   <si>
     <t>Type</t>
   </si>
@@ -456,9 +456,6 @@
     <t>Unused</t>
   </si>
   <si>
-    <t>Min/Max from Kris' email 8/29/2014</t>
-  </si>
-  <si>
     <t>Max value only constrained by data type</t>
   </si>
   <si>
@@ -736,6 +733,9 @@
   </si>
   <si>
     <t>If true, colony dies when pollen or nectar mass reaches 0</t>
+  </si>
+  <si>
+    <t>Min/Max from Kris' email 8/29/2014; modified by Jeff to include neonicotinoids</t>
   </si>
 </sst>
 </file>
@@ -1094,23 +1094,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130:G131"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.62890625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="37.62890625" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="13.9453125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.47265625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.5234375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="42.62890625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="78.68359375" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.83984375" style="3"/>
+    <col min="1" max="1" width="37.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="78.7109375" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1118,7 +1118,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="17.7" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>139</v>
       </c>
@@ -1138,10 +1138,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1156,13 +1156,13 @@
         <v>58</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1180,10 +1180,10 @@
         <v>143</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1201,10 +1201,10 @@
         <v>143</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1216,13 +1216,13 @@
         <v>0</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1234,13 +1234,13 @@
         <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1252,13 +1252,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1270,13 +1270,13 @@
         <v>0</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1288,13 +1288,13 @@
         <v>0</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1306,13 +1306,13 @@
         <v>0</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1324,13 +1324,13 @@
         <v>0</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1342,13 +1342,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1363,10 +1363,10 @@
         <v>5</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1381,10 +1381,10 @@
         <v>16</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1399,10 +1399,10 @@
         <v>100</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1417,10 +1417,10 @@
         <v>100</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1432,10 +1432,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1450,10 +1450,10 @@
         <v>100</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1468,10 +1468,10 @@
         <v>100</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1486,10 +1486,10 @@
         <v>100</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1504,10 +1504,10 @@
         <v>100</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1522,10 +1522,10 @@
         <v>100</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1543,10 +1543,10 @@
         <v>29</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1564,10 +1564,10 @@
         <v>29</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1585,10 +1585,10 @@
         <v>29</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1606,10 +1606,10 @@
         <v>29</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -1627,10 +1627,10 @@
         <v>29</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -1648,10 +1648,10 @@
         <v>29</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1669,10 +1669,10 @@
         <v>29</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1690,10 +1690,10 @@
         <v>29</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -1711,10 +1711,10 @@
         <v>29</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -1732,10 +1732,10 @@
         <v>29</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -1753,10 +1753,10 @@
         <v>29</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -1774,10 +1774,10 @@
         <v>29</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -1795,10 +1795,10 @@
         <v>29</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -1816,10 +1816,10 @@
         <v>29</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1837,10 +1837,10 @@
         <v>29</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>45</v>
       </c>
@@ -1858,10 +1858,10 @@
         <v>29</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>46</v>
       </c>
@@ -1879,10 +1879,10 @@
         <v>29</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>47</v>
       </c>
@@ -1900,10 +1900,10 @@
         <v>29</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>48</v>
       </c>
@@ -1921,10 +1921,10 @@
         <v>29</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>49</v>
       </c>
@@ -1942,10 +1942,10 @@
         <v>29</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
@@ -1963,10 +1963,10 @@
         <v>29</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>51</v>
       </c>
@@ -1984,10 +1984,10 @@
         <v>29</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>52</v>
       </c>
@@ -2005,10 +2005,10 @@
         <v>29</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.5">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>53</v>
       </c>
@@ -2026,10 +2026,10 @@
         <v>29</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.5">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
@@ -2047,10 +2047,10 @@
         <v>29</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.5">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>59</v>
       </c>
@@ -2068,10 +2068,10 @@
         <v>141</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.5">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
@@ -2083,13 +2083,13 @@
         <v>0</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.5">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>60</v>
       </c>
@@ -2104,10 +2104,10 @@
         <v>100</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.5">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>61</v>
       </c>
@@ -2125,10 +2125,10 @@
         <v>143</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>62</v>
       </c>
@@ -2146,10 +2146,10 @@
         <v>143</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>63</v>
       </c>
@@ -2167,10 +2167,10 @@
         <v>29</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.5">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>64</v>
       </c>
@@ -2182,13 +2182,13 @@
         <v>0</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.5">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>66</v>
       </c>
@@ -2227,10 +2227,10 @@
         <v>143</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.5">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>67</v>
       </c>
@@ -2248,10 +2248,10 @@
         <v>29</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.5">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>68</v>
       </c>
@@ -2269,10 +2269,10 @@
         <v>29</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.5">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>69</v>
       </c>
@@ -2287,10 +2287,10 @@
         <v>5</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.5">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>70</v>
       </c>
@@ -2308,10 +2308,10 @@
         <v>29</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.5">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>71</v>
       </c>
@@ -2323,10 +2323,10 @@
         <v>1</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.5">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>72</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>73</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>74</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>75</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>76</v>
       </c>
@@ -2401,16 +2401,16 @@
         <v>23</v>
       </c>
       <c r="D67" s="4">
-        <v>-9</v>
+        <v>1</v>
       </c>
       <c r="E67" s="4">
-        <v>-2</v>
+        <v>9</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>77</v>
       </c>
@@ -2419,16 +2419,16 @@
         <v>23</v>
       </c>
       <c r="D68" s="4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="E68" s="4">
         <v>100</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>78</v>
       </c>
@@ -2437,16 +2437,16 @@
         <v>23</v>
       </c>
       <c r="D69" s="4">
-        <v>-9</v>
+        <v>1</v>
       </c>
       <c r="E69" s="4">
-        <v>-2</v>
+        <v>9</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>79</v>
       </c>
@@ -2455,16 +2455,16 @@
         <v>23</v>
       </c>
       <c r="D70" s="4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="E70" s="4">
         <v>100</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>80</v>
       </c>
@@ -2473,16 +2473,16 @@
         <v>23</v>
       </c>
       <c r="D71" s="4">
-        <v>-9</v>
+        <v>1</v>
       </c>
       <c r="E71" s="4">
-        <v>-2</v>
+        <v>9</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>81</v>
       </c>
@@ -2491,16 +2491,16 @@
         <v>23</v>
       </c>
       <c r="D72" s="4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="E72" s="4">
         <v>100</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>82</v>
       </c>
@@ -2515,10 +2515,10 @@
         <v>1000000</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>83</v>
       </c>
@@ -2533,10 +2533,10 @@
         <v>10000</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>84</v>
       </c>
@@ -2550,11 +2550,8 @@
       <c r="E75" s="4">
         <v>35</v>
       </c>
-      <c r="F75" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.5">
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>85</v>
       </c>
@@ -2563,10 +2560,10 @@
         <v>23</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.5">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>86</v>
       </c>
@@ -2578,13 +2575,13 @@
         <v>0</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.5">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>87</v>
       </c>
@@ -2596,13 +2593,13 @@
         <v>0</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.5">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>88</v>
       </c>
@@ -2614,13 +2611,13 @@
         <v>0</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.5">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>89</v>
       </c>
@@ -2632,13 +2629,13 @@
         <v>0</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>90</v>
       </c>
@@ -2650,13 +2647,13 @@
         <v>0</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.5">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>91</v>
       </c>
@@ -2668,13 +2665,13 @@
         <v>0</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.5">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>92</v>
       </c>
@@ -2686,13 +2683,13 @@
         <v>0</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>93</v>
       </c>
@@ -2704,13 +2701,13 @@
         <v>0</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.5">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>94</v>
       </c>
@@ -2722,13 +2719,13 @@
         <v>0</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.5">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>95</v>
       </c>
@@ -2740,13 +2737,13 @@
         <v>0</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.5">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>96</v>
       </c>
@@ -2758,13 +2755,13 @@
         <v>0</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.5">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>97</v>
       </c>
@@ -2776,13 +2773,13 @@
         <v>0</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.5">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>98</v>
       </c>
@@ -2794,13 +2791,13 @@
         <v>0</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.5">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>99</v>
       </c>
@@ -2812,13 +2809,13 @@
         <v>0</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.5">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>100</v>
       </c>
@@ -2830,13 +2827,13 @@
         <v>0</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.5">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>101</v>
       </c>
@@ -2848,13 +2845,13 @@
         <v>0</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.5">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>102</v>
       </c>
@@ -2866,13 +2863,13 @@
         <v>0</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.5">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>103</v>
       </c>
@@ -2884,13 +2881,13 @@
         <v>0</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>104</v>
       </c>
@@ -2905,10 +2902,10 @@
         <v>100</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.5">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>105</v>
       </c>
@@ -2920,13 +2917,13 @@
         <v>0</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.5">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>106</v>
       </c>
@@ -2938,13 +2935,13 @@
         <v>0</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.5">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>107</v>
       </c>
@@ -2962,10 +2959,10 @@
         <v>29</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.5">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>108</v>
       </c>
@@ -2983,10 +2980,10 @@
         <v>29</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.5">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>109</v>
       </c>
@@ -3004,10 +3001,10 @@
         <v>29</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.5">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>110</v>
       </c>
@@ -3019,10 +3016,10 @@
         <v>0</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.5">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>111</v>
       </c>
@@ -3034,10 +3031,10 @@
         <v>0</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.5">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>112</v>
       </c>
@@ -3052,7 +3049,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>113</v>
       </c>
@@ -3067,7 +3064,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>114</v>
       </c>
@@ -3079,10 +3076,10 @@
         <v>0</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.5">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>115</v>
       </c>
@@ -3094,10 +3091,10 @@
         <v>0</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.5">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>116</v>
       </c>
@@ -3115,10 +3112,10 @@
         <v>143</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.5">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>117</v>
       </c>
@@ -3136,7 +3133,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>118</v>
       </c>
@@ -3154,7 +3151,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>119</v>
       </c>
@@ -3172,7 +3169,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>120</v>
       </c>
@@ -3190,7 +3187,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>121</v>
       </c>
@@ -3208,7 +3205,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>122</v>
       </c>
@@ -3226,7 +3223,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>123</v>
       </c>
@@ -3244,10 +3241,10 @@
         <v>29</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.5">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>124</v>
       </c>
@@ -3262,13 +3259,13 @@
         <v>58</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.5">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>125</v>
       </c>
@@ -3280,13 +3277,13 @@
         <v>0</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.5">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>126</v>
       </c>
@@ -3298,13 +3295,13 @@
         <v>0</v>
       </c>
       <c r="F117" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.5">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>127</v>
       </c>
@@ -3316,13 +3313,13 @@
         <v>0</v>
       </c>
       <c r="F118" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.5">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>128</v>
       </c>
@@ -3334,13 +3331,13 @@
         <v>0</v>
       </c>
       <c r="F119" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.5">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>129</v>
       </c>
@@ -3358,10 +3355,10 @@
         <v>29</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.5">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>130</v>
       </c>
@@ -3373,13 +3370,13 @@
         <v>0</v>
       </c>
       <c r="F121" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.5">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>131</v>
       </c>
@@ -3397,10 +3394,10 @@
         <v>143</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.5">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>132</v>
       </c>
@@ -3418,10 +3415,10 @@
         <v>143</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.5">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>133</v>
       </c>
@@ -3439,10 +3436,10 @@
         <v>29</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.5">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>134</v>
       </c>
@@ -3454,13 +3451,13 @@
         <v>0</v>
       </c>
       <c r="F125" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.5">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>135</v>
       </c>
@@ -3478,10 +3475,10 @@
         <v>143</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.5">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>136</v>
       </c>
@@ -3499,10 +3496,10 @@
         <v>143</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.5">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>137</v>
       </c>
@@ -3517,10 +3514,10 @@
         <v>1</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.5">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>138</v>
       </c>
@@ -3538,22 +3535,22 @@
         <v>29</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.5">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
     </row>

</xml_diff>